<commit_message>
added new configureation and corrected theory and state-of-the-art chapter
</commit_message>
<xml_diff>
--- a/dtpu_configurations/only_integer8/120mhz/mxu_3x3/power.xlsx
+++ b/dtpu_configurations/only_integer8/120mhz/mxu_3x3/power.xlsx
@@ -175,34 +175,34 @@
         <v>11</v>
       </c>
       <c r="B2" t="n" s="4">
-        <v>0.045201729983091354</v>
+        <v>0.04710838198661804</v>
       </c>
       <c r="C2" t="n" s="4">
-        <v>0.022686541080474854</v>
+        <v>0.019473830237984657</v>
       </c>
       <c r="D2" t="n" s="4">
-        <v>0.016221560537815094</v>
+        <v>0.015438690781593323</v>
       </c>
       <c r="E2" t="n" s="4">
-        <v>0.008203281089663506</v>
+        <v>0.00775632169097662</v>
       </c>
       <c r="F2" t="n" s="4">
-        <v>7.46409386920277E-6</v>
+        <v>7.074088443914661E-6</v>
       </c>
       <c r="G2" t="n" s="4">
-        <v>0.0026751323603093624</v>
+        <v>0.002529376884922385</v>
       </c>
       <c r="H2" t="n" s="4">
-        <v>0.0024250000715255737</v>
+        <v>0.002292873105034232</v>
       </c>
       <c r="I2" t="n" s="4">
-        <v>1.263510823249817</v>
+        <v>1.2630733251571655</v>
       </c>
       <c r="J2" t="n" s="4">
-        <v>0.1257345825433731</v>
+        <v>0.12570902705192566</v>
       </c>
       <c r="K2" t="n" s="4">
-        <v>1.4866825342178345</v>
+        <v>1.4834043979644775</v>
       </c>
     </row>
   </sheetData>

</xml_diff>